<commit_message>
Ver-3.0.0 1. Methods for individual metrics have been changed. 2. Methods for centrality metrics of single graphs have been added.
</commit_message>
<xml_diff>
--- a/result/Astronomy_indiv.xlsx
+++ b/result/Astronomy_indiv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,40 +451,35 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>num_of_hierarchies</t>
+          <t>num_of_crosslinks</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>num_of_crosslinks</t>
+          <t>ASPL</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ASPL</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>network_density</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>network_density</t>
+          <t>complexity</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>complexity</t>
+          <t>level_of_deepest_hierarchy</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>level_of_deepest_hierarchy</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>num_of_components</t>
         </is>
@@ -503,27 +498,24 @@
         <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2.266666666666667</v>
       </c>
       <c r="F2" t="n">
-        <v>2.266666666666667</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.06190476190476191</v>
       </c>
       <c r="H2" t="n">
-        <v>0.06190476190476191</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8666666666666667</v>
+        <v>3</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -540,27 +532,24 @@
         <v>49</v>
       </c>
       <c r="D3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.691954022988506</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1378333333333333</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.05632183908045977</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.633333333333333</v>
+      </c>
+      <c r="I3" t="n">
         <v>4</v>
       </c>
-      <c r="E3" t="n">
-        <v>16</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3.691954022988506</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.1378333333333333</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.05632183908045977</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.633333333333333</v>
-      </c>
       <c r="J3" t="n">
-        <v>4</v>
-      </c>
-      <c r="K3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -577,27 +566,24 @@
         <v>48</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>5.588588588588588</v>
       </c>
       <c r="F4" t="n">
-        <v>5.588588588588588</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0341394025604552</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0341394025604552</v>
+        <v>1.263157894736842</v>
       </c>
       <c r="I4" t="n">
-        <v>1.263157894736842</v>
+        <v>9</v>
       </c>
       <c r="J4" t="n">
-        <v>9</v>
-      </c>
-      <c r="K4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -614,27 +600,24 @@
         <v>25</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>2.882352941176471</v>
       </c>
       <c r="F5" t="n">
-        <v>2.882352941176471</v>
+        <v>0.06013071895424836</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06013071895424836</v>
+        <v>0.09191176470588236</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09191176470588236</v>
+        <v>1.470588235294118</v>
       </c>
       <c r="I5" t="n">
-        <v>1.470588235294118</v>
+        <v>6</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -651,27 +634,24 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.186813186813187</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.05714285714285715</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.08241758241758242</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.071428571428571</v>
+      </c>
+      <c r="I6" t="n">
         <v>5</v>
       </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3.186813186813187</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.05714285714285715</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.08241758241758242</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.071428571428571</v>
-      </c>
       <c r="J6" t="n">
-        <v>5</v>
-      </c>
-      <c r="K6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -688,27 +668,24 @@
         <v>31</v>
       </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.661290322580645</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.96875</v>
+      </c>
+      <c r="I7" t="n">
         <v>5</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.661290322580645</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.03125</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.96875</v>
-      </c>
       <c r="J7" t="n">
-        <v>5</v>
-      </c>
-      <c r="K7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -725,27 +702,24 @@
         <v>38</v>
       </c>
       <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.14021164021164</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.05026455026455026</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.357142857142857</v>
+      </c>
+      <c r="I8" t="n">
         <v>5</v>
       </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>4.14021164021164</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.05026455026455026</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1.357142857142857</v>
-      </c>
       <c r="J8" t="n">
-        <v>5</v>
-      </c>
-      <c r="K8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -762,27 +736,24 @@
         <v>50</v>
       </c>
       <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.024193548387097</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.03440504807692307</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.05040322580645161</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.5625</v>
+      </c>
+      <c r="I9" t="n">
         <v>8</v>
       </c>
-      <c r="E9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" t="n">
-        <v>4.024193548387097</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.03440504807692307</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.05040322580645161</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.5625</v>
-      </c>
       <c r="J9" t="n">
-        <v>8</v>
-      </c>
-      <c r="K9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -799,27 +770,24 @@
         <v>33</v>
       </c>
       <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.644268774703557</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1290149640626841</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.06521739130434782</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.434782608695652</v>
+      </c>
+      <c r="I10" t="n">
         <v>5</v>
       </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3.644268774703557</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.1290149640626841</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.06521739130434782</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1.434782608695652</v>
-      </c>
       <c r="J10" t="n">
-        <v>5</v>
-      </c>
-      <c r="K10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -836,27 +804,24 @@
         <v>45</v>
       </c>
       <c r="D11" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.615384615384615</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.254320987654321</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0641025641025641</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="I11" t="n">
         <v>5</v>
       </c>
-      <c r="E11" t="n">
-        <v>11</v>
-      </c>
-      <c r="F11" t="n">
-        <v>3.615384615384615</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.254320987654321</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.0641025641025641</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1.666666666666667</v>
-      </c>
       <c r="J11" t="n">
-        <v>5</v>
-      </c>
-      <c r="K11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -873,27 +838,24 @@
         <v>55</v>
       </c>
       <c r="D12" t="n">
+        <v>16</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.978662873399716</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.09736842105263159</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.03911806543385491</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.447368421052632</v>
+      </c>
+      <c r="I12" t="n">
         <v>5</v>
       </c>
-      <c r="E12" t="n">
-        <v>16</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3.978662873399716</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.09736842105263159</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.03911806543385491</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1.447368421052632</v>
-      </c>
       <c r="J12" t="n">
-        <v>5</v>
-      </c>
-      <c r="K12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -910,27 +872,24 @@
         <v>122</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E13" t="n">
-        <v>26</v>
+        <v>5.612159329140461</v>
       </c>
       <c r="F13" t="n">
-        <v>5.612159329140461</v>
+        <v>0.04117204811649255</v>
       </c>
       <c r="G13" t="n">
-        <v>0.04117204811649255</v>
+        <v>0.04262753319357093</v>
       </c>
       <c r="H13" t="n">
-        <v>0.04262753319357093</v>
+        <v>2.259259259259259</v>
       </c>
       <c r="I13" t="n">
-        <v>2.259259259259259</v>
+        <v>13</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -947,29 +906,26 @@
         <v>26</v>
       </c>
       <c r="D14" t="n">
-        <v>2.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>2.407662835249042</v>
       </c>
       <c r="F14" t="n">
-        <v>2.407662835249042</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.03201970443349754</v>
       </c>
       <c r="H14" t="n">
-        <v>0.03201970443349754</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="I14" t="n">
-        <v>0.896551724137931</v>
+        <v>3</v>
       </c>
       <c r="J14" t="n">
         <v>3</v>
       </c>
-      <c r="K14" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -984,27 +940,24 @@
         <v>28</v>
       </c>
       <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.750988142292491</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.1434782608695652</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.05533596837944664</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.217391304347826</v>
+      </c>
+      <c r="I15" t="n">
         <v>5</v>
       </c>
-      <c r="E15" t="n">
-        <v>6</v>
-      </c>
-      <c r="F15" t="n">
-        <v>3.750988142292491</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.1434782608695652</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.05533596837944664</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1.217391304347826</v>
-      </c>
       <c r="J15" t="n">
-        <v>5</v>
-      </c>
-      <c r="K15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1021,27 +974,24 @@
         <v>53</v>
       </c>
       <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.522689075630252</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.04453781512605042</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.514285714285714</v>
+      </c>
+      <c r="I16" t="n">
         <v>4</v>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>3.522689075630252</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.04453781512605042</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1.514285714285714</v>
-      </c>
       <c r="J16" t="n">
-        <v>4</v>
-      </c>
-      <c r="K16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1058,27 +1008,24 @@
         <v>31</v>
       </c>
       <c r="D17" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>2.484420928865374</v>
       </c>
       <c r="F17" t="n">
-        <v>2.484420928865374</v>
+        <v>0.0382716049382716</v>
       </c>
       <c r="G17" t="n">
-        <v>0.06458333333333333</v>
+        <v>0.04415954415954416</v>
       </c>
       <c r="H17" t="n">
-        <v>0.04415954415954416</v>
+        <v>1.148148148148148</v>
       </c>
       <c r="I17" t="n">
-        <v>1.148148148148148</v>
+        <v>3</v>
       </c>
       <c r="J17" t="n">
-        <v>4</v>
-      </c>
-      <c r="K17" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1095,27 +1042,24 @@
         <v>34</v>
       </c>
       <c r="D18" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>3.018279569892473</v>
       </c>
       <c r="F18" t="n">
-        <v>3.018279569892473</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.03655913978494624</v>
       </c>
       <c r="H18" t="n">
-        <v>0.03655913978494624</v>
+        <v>1.096774193548387</v>
       </c>
       <c r="I18" t="n">
-        <v>1.096774193548387</v>
+        <v>6</v>
       </c>
       <c r="J18" t="n">
-        <v>6</v>
-      </c>
-      <c r="K18" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1132,27 +1076,24 @@
         <v>23</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>2.647342995169082</v>
       </c>
       <c r="F19" t="n">
-        <v>2.647342995169082</v>
+        <v>0.0608695652173913</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03684210526315789</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04545454545454546</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J19" t="n">
-        <v>4</v>
-      </c>
-      <c r="K19" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1169,27 +1110,24 @@
         <v>66</v>
       </c>
       <c r="D20" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4.533333333333333</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.03329339143064634</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.466666666666667</v>
+      </c>
+      <c r="I20" t="n">
         <v>7</v>
       </c>
-      <c r="E20" t="n">
-        <v>4</v>
-      </c>
-      <c r="F20" t="n">
-        <v>4.533333333333333</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.03329339143064634</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.03333333333333333</v>
-      </c>
-      <c r="I20" t="n">
-        <v>1.466666666666667</v>
-      </c>
       <c r="J20" t="n">
-        <v>7</v>
-      </c>
-      <c r="K20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1206,27 +1144,24 @@
         <v>30</v>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>3.574712643678161</v>
       </c>
       <c r="F21" t="n">
-        <v>3.574712643678161</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.03448275862068965</v>
       </c>
       <c r="H21" t="n">
-        <v>0.03448275862068965</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J21" t="n">
-        <v>4</v>
-      </c>
-      <c r="K21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1243,27 +1178,24 @@
         <v>25</v>
       </c>
       <c r="D22" t="n">
-        <v>2.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2.601809954751132</v>
       </c>
       <c r="F22" t="n">
-        <v>2.601809954751132</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.03846153846153846</v>
       </c>
       <c r="H22" t="n">
-        <v>0.03846153846153846</v>
+        <v>0.9615384615384616</v>
       </c>
       <c r="I22" t="n">
-        <v>0.9615384615384616</v>
+        <v>4</v>
       </c>
       <c r="J22" t="n">
-        <v>4</v>
-      </c>
-      <c r="K22" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1280,27 +1212,24 @@
         <v>69</v>
       </c>
       <c r="D23" t="n">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.289907157831686</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.02503628447024673</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.30188679245283</v>
+      </c>
+      <c r="I23" t="n">
         <v>4</v>
       </c>
-      <c r="E23" t="n">
-        <v>8</v>
-      </c>
-      <c r="F23" t="n">
-        <v>3.289907157831686</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.02503628447024673</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1.30188679245283</v>
-      </c>
       <c r="J23" t="n">
-        <v>4</v>
-      </c>
-      <c r="K23" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1317,27 +1246,24 @@
         <v>61</v>
       </c>
       <c r="D24" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E24" t="n">
-        <v>14</v>
+        <v>4.061428571428571</v>
       </c>
       <c r="F24" t="n">
-        <v>4.061428571428571</v>
+        <v>0.04682234432234432</v>
       </c>
       <c r="G24" t="n">
-        <v>0.02601241351241351</v>
+        <v>0.0391025641025641</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0391025641025641</v>
+        <v>1.525</v>
       </c>
       <c r="I24" t="n">
-        <v>1.525</v>
+        <v>6</v>
       </c>
       <c r="J24" t="n">
-        <v>6</v>
-      </c>
-      <c r="K24" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1354,27 +1280,24 @@
         <v>43</v>
       </c>
       <c r="D25" t="n">
-        <v>3.333333333333333</v>
+        <v>9</v>
       </c>
       <c r="E25" t="n">
-        <v>9</v>
+        <v>2.854700854700855</v>
       </c>
       <c r="F25" t="n">
-        <v>2.854700854700855</v>
+        <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.03412698412698412</v>
       </c>
       <c r="H25" t="n">
-        <v>0.03412698412698412</v>
+        <v>1.194444444444444</v>
       </c>
       <c r="I25" t="n">
-        <v>1.194444444444444</v>
+        <v>4</v>
       </c>
       <c r="J25" t="n">
-        <v>4</v>
-      </c>
-      <c r="K25" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1391,27 +1314,24 @@
         <v>23</v>
       </c>
       <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.517786561264822</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.04545454545454546</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
         <v>6</v>
       </c>
-      <c r="E26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" t="n">
-        <v>3.517786561264822</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.04545454545454546</v>
-      </c>
-      <c r="I26" t="n">
-        <v>1</v>
-      </c>
       <c r="J26" t="n">
-        <v>6</v>
-      </c>
-      <c r="K26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1428,27 +1348,24 @@
         <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>2.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>2.996894409937888</v>
       </c>
       <c r="F27" t="n">
-        <v>2.996894409937888</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.03201970443349754</v>
       </c>
       <c r="H27" t="n">
-        <v>0.03201970443349754</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="I27" t="n">
-        <v>0.896551724137931</v>
+        <v>4</v>
       </c>
       <c r="J27" t="n">
-        <v>4</v>
-      </c>
-      <c r="K27" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1465,27 +1382,24 @@
         <v>44</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E28" t="n">
-        <v>14</v>
+        <v>2.535353535353535</v>
       </c>
       <c r="F28" t="n">
-        <v>2.535353535353535</v>
+        <v>0.0821324354657688</v>
       </c>
       <c r="G28" t="n">
-        <v>0.04820816864295126</v>
+        <v>0.06267806267806268</v>
       </c>
       <c r="H28" t="n">
-        <v>0.06267806267806268</v>
+        <v>1.62962962962963</v>
       </c>
       <c r="I28" t="n">
-        <v>1.62962962962963</v>
+        <v>4</v>
       </c>
       <c r="J28" t="n">
-        <v>2</v>
-      </c>
-      <c r="K28" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1502,27 +1416,24 @@
         <v>68</v>
       </c>
       <c r="D29" t="n">
+        <v>9</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4.562626262626263</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.06074074074074074</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.03434343434343434</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.511111111111111</v>
+      </c>
+      <c r="I29" t="n">
         <v>7</v>
       </c>
-      <c r="E29" t="n">
-        <v>9</v>
-      </c>
-      <c r="F29" t="n">
-        <v>4.562626262626263</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.06074074074074074</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.03434343434343434</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1.511111111111111</v>
-      </c>
       <c r="J29" t="n">
-        <v>7</v>
-      </c>
-      <c r="K29" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1539,27 +1450,24 @@
         <v>57</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>3.586206896551724</v>
       </c>
       <c r="F30" t="n">
-        <v>3.586206896551724</v>
+        <v>0.02368421052631579</v>
       </c>
       <c r="G30" t="n">
-        <v>0.02368421052631579</v>
+        <v>0.06551724137931035</v>
       </c>
       <c r="H30" t="n">
-        <v>0.06551724137931035</v>
+        <v>1.9</v>
       </c>
       <c r="I30" t="n">
-        <v>1.9</v>
+        <v>5</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
-      </c>
-      <c r="K30" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1576,27 +1484,24 @@
         <v>18</v>
       </c>
       <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.125</v>
+      </c>
+      <c r="I31" t="n">
         <v>3</v>
       </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>2.35</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="I31" t="n">
-        <v>1.125</v>
-      </c>
       <c r="J31" t="n">
-        <v>3</v>
-      </c>
-      <c r="K31" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1613,27 +1518,24 @@
         <v>57</v>
       </c>
       <c r="D32" t="n">
+        <v>25</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.55026455026455</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.2761316581933081</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.07539682539682539</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2.035714285714286</v>
+      </c>
+      <c r="I32" t="n">
         <v>6</v>
       </c>
-      <c r="E32" t="n">
-        <v>25</v>
-      </c>
-      <c r="F32" t="n">
-        <v>2.55026455026455</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.2761316581933081</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.07539682539682539</v>
-      </c>
-      <c r="I32" t="n">
-        <v>2.035714285714286</v>
-      </c>
       <c r="J32" t="n">
-        <v>6</v>
-      </c>
-      <c r="K32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1650,27 +1552,24 @@
         <v>52</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E33" t="n">
-        <v>13</v>
+        <v>3.413547237076649</v>
       </c>
       <c r="F33" t="n">
-        <v>3.413547237076649</v>
+        <v>0.03202614379084968</v>
       </c>
       <c r="G33" t="n">
-        <v>0.03202614379084968</v>
+        <v>0.04634581105169341</v>
       </c>
       <c r="H33" t="n">
-        <v>0.04634581105169341</v>
+        <v>1.529411764705882</v>
       </c>
       <c r="I33" t="n">
-        <v>1.529411764705882</v>
+        <v>6</v>
       </c>
       <c r="J33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1687,29 +1586,26 @@
         <v>28</v>
       </c>
       <c r="D34" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1.987577639751553</v>
       </c>
       <c r="F34" t="n">
-        <v>1.987577639751553</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>0.05533596837944664</v>
       </c>
       <c r="H34" t="n">
-        <v>0.05533596837944664</v>
+        <v>1.217391304347826</v>
       </c>
       <c r="I34" t="n">
-        <v>1.217391304347826</v>
+        <v>3</v>
       </c>
       <c r="J34" t="n">
         <v>4</v>
       </c>
-      <c r="K34" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -1724,27 +1620,24 @@
         <v>92</v>
       </c>
       <c r="D35" t="n">
+        <v>24</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.89608636977058</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.0620782726045884</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2.358974358974359</v>
+      </c>
+      <c r="I35" t="n">
         <v>6</v>
       </c>
-      <c r="E35" t="n">
-        <v>24</v>
-      </c>
-      <c r="F35" t="n">
-        <v>3.89608636977058</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.0620782726045884</v>
-      </c>
-      <c r="I35" t="n">
-        <v>2.358974358974359</v>
-      </c>
       <c r="J35" t="n">
-        <v>6</v>
-      </c>
-      <c r="K35" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1764,24 +1657,21 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>4.524893314366999</v>
       </c>
       <c r="F36" t="n">
-        <v>4.524893314366999</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>0.04409672830725463</v>
       </c>
       <c r="H36" t="n">
-        <v>0.04409672830725463</v>
+        <v>1.631578947368421</v>
       </c>
       <c r="I36" t="n">
-        <v>1.631578947368421</v>
+        <v>6</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
-      </c>
-      <c r="K36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1798,27 +1688,24 @@
         <v>40</v>
       </c>
       <c r="D37" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>3.184523809523809</v>
       </c>
       <c r="F37" t="n">
-        <v>3.184523809523809</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>0.02322880371660859</v>
       </c>
       <c r="H37" t="n">
-        <v>0.02322880371660859</v>
+        <v>0.9523809523809523</v>
       </c>
       <c r="I37" t="n">
-        <v>0.9523809523809523</v>
+        <v>4</v>
       </c>
       <c r="J37" t="n">
-        <v>4</v>
-      </c>
-      <c r="K37" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1835,27 +1722,24 @@
         <v>61</v>
       </c>
       <c r="D38" t="n">
+        <v>11</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.034574468085107</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.04101130351130352</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.02703900709219858</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.270833333333333</v>
+      </c>
+      <c r="I38" t="n">
         <v>6</v>
       </c>
-      <c r="E38" t="n">
-        <v>11</v>
-      </c>
-      <c r="F38" t="n">
-        <v>4.034574468085107</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.04101130351130352</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.02703900709219858</v>
-      </c>
-      <c r="I38" t="n">
-        <v>1.270833333333333</v>
-      </c>
       <c r="J38" t="n">
-        <v>6</v>
-      </c>
-      <c r="K38" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1872,27 +1756,24 @@
         <v>65</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>4.310283687943262</v>
       </c>
       <c r="F39" t="n">
-        <v>4.310283687943262</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>0.02881205673758865</v>
       </c>
       <c r="H39" t="n">
-        <v>0.02881205673758865</v>
+        <v>1.354166666666667</v>
       </c>
       <c r="I39" t="n">
-        <v>1.354166666666667</v>
+        <v>5</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
-      </c>
-      <c r="K39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1909,27 +1790,24 @@
         <v>31</v>
       </c>
       <c r="D40" t="n">
+        <v>6</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2.876666666666666</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.1150338983050847</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.05166666666666667</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="I40" t="n">
         <v>5</v>
       </c>
-      <c r="E40" t="n">
-        <v>6</v>
-      </c>
-      <c r="F40" t="n">
-        <v>2.876666666666666</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0.1150338983050847</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0.05166666666666667</v>
-      </c>
-      <c r="I40" t="n">
-        <v>1.24</v>
-      </c>
       <c r="J40" t="n">
-        <v>5</v>
-      </c>
-      <c r="K40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1946,27 +1824,24 @@
         <v>30</v>
       </c>
       <c r="D41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.310344827586207</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.03694581280788178</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1.03448275862069</v>
+      </c>
+      <c r="I41" t="n">
         <v>4</v>
       </c>
-      <c r="E41" t="n">
-        <v>2</v>
-      </c>
-      <c r="F41" t="n">
-        <v>3.310344827586207</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0.03694581280788178</v>
-      </c>
-      <c r="I41" t="n">
-        <v>1.03448275862069</v>
-      </c>
       <c r="J41" t="n">
-        <v>4</v>
-      </c>
-      <c r="K41" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1983,27 +1858,24 @@
         <v>79</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>3.290455576169862</v>
       </c>
       <c r="F42" t="n">
-        <v>3.290455576169862</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>0.04587688734030197</v>
       </c>
       <c r="H42" t="n">
-        <v>0.04587688734030197</v>
+        <v>1.880952380952381</v>
       </c>
       <c r="I42" t="n">
-        <v>1.880952380952381</v>
+        <v>4</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
-      </c>
-      <c r="K42" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2020,27 +1892,24 @@
         <v>36</v>
       </c>
       <c r="D43" t="n">
-        <v>3.5</v>
+        <v>14</v>
       </c>
       <c r="E43" t="n">
-        <v>14</v>
+        <v>2.628472222222222</v>
       </c>
       <c r="F43" t="n">
-        <v>2.628472222222222</v>
+        <v>0.1236111111111111</v>
       </c>
       <c r="G43" t="n">
-        <v>0.08725490196078432</v>
+        <v>0.06521739130434782</v>
       </c>
       <c r="H43" t="n">
-        <v>0.06521739130434782</v>
+        <v>1.5</v>
       </c>
       <c r="I43" t="n">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="J43" t="n">
-        <v>4</v>
-      </c>
-      <c r="K43" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2060,24 +1929,21 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>2.190476190476191</v>
       </c>
       <c r="F44" t="n">
-        <v>2.190476190476191</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="H44" t="n">
-        <v>0.2142857142857143</v>
+        <v>1.285714285714286</v>
       </c>
       <c r="I44" t="n">
-        <v>1.285714285714286</v>
+        <v>3</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
-      </c>
-      <c r="K44" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2094,27 +1960,24 @@
         <v>34</v>
       </c>
       <c r="D45" t="n">
-        <v>3.666666666666667</v>
+        <v>7</v>
       </c>
       <c r="E45" t="n">
+        <v>3.965608465608466</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.04497354497354497</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1.214285714285714</v>
+      </c>
+      <c r="I45" t="n">
         <v>7</v>
       </c>
-      <c r="F45" t="n">
-        <v>3.965608465608466</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0.04497354497354497</v>
-      </c>
-      <c r="I45" t="n">
-        <v>1.214285714285714</v>
-      </c>
       <c r="J45" t="n">
-        <v>7</v>
-      </c>
-      <c r="K45" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2131,27 +1994,24 @@
         <v>19</v>
       </c>
       <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.176470588235294</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.02654320987654321</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.06209150326797386</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1.055555555555556</v>
+      </c>
+      <c r="I46" t="n">
         <v>5</v>
       </c>
-      <c r="E46" t="n">
-        <v>2</v>
-      </c>
-      <c r="F46" t="n">
-        <v>3.176470588235294</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.02654320987654321</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.06209150326797386</v>
-      </c>
-      <c r="I46" t="n">
-        <v>1.055555555555556</v>
-      </c>
       <c r="J46" t="n">
-        <v>5</v>
-      </c>
-      <c r="K46" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2168,27 +2028,24 @@
         <v>42</v>
       </c>
       <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.695767195767196</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.00865079365079365</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I47" t="n">
         <v>5</v>
       </c>
-      <c r="E47" t="n">
-        <v>2</v>
-      </c>
-      <c r="F47" t="n">
-        <v>3.695767195767196</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.00865079365079365</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="I47" t="n">
-        <v>1.5</v>
-      </c>
       <c r="J47" t="n">
-        <v>5</v>
-      </c>
-      <c r="K47" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2205,27 +2062,24 @@
         <v>14</v>
       </c>
       <c r="D48" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>2.742857142857143</v>
       </c>
       <c r="F48" t="n">
-        <v>2.742857142857143</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>0.05833333333333333</v>
       </c>
       <c r="H48" t="n">
-        <v>0.05833333333333333</v>
+        <v>0.875</v>
       </c>
       <c r="I48" t="n">
-        <v>0.875</v>
+        <v>4</v>
       </c>
       <c r="J48" t="n">
-        <v>4</v>
-      </c>
-      <c r="K48" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2242,27 +2096,24 @@
         <v>47</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E49" t="n">
-        <v>14</v>
+        <v>4.163306451612903</v>
       </c>
       <c r="F49" t="n">
-        <v>4.163306451612903</v>
+        <v>0.08171706309041835</v>
       </c>
       <c r="G49" t="n">
-        <v>0.08171706309041835</v>
+        <v>0.04737903225806452</v>
       </c>
       <c r="H49" t="n">
-        <v>0.04737903225806452</v>
+        <v>1.46875</v>
       </c>
       <c r="I49" t="n">
-        <v>1.46875</v>
+        <v>6</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
-      </c>
-      <c r="K49" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2279,27 +2130,24 @@
         <v>59</v>
       </c>
       <c r="D50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" t="n">
+        <v>4.62051282051282</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.03782051282051282</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1.475</v>
+      </c>
+      <c r="I50" t="n">
         <v>6</v>
       </c>
-      <c r="E50" t="n">
-        <v>2</v>
-      </c>
-      <c r="F50" t="n">
-        <v>4.62051282051282</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.03782051282051282</v>
-      </c>
-      <c r="I50" t="n">
-        <v>1.475</v>
-      </c>
       <c r="J50" t="n">
-        <v>6</v>
-      </c>
-      <c r="K50" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2316,27 +2164,24 @@
         <v>21</v>
       </c>
       <c r="D51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>2.886904761904762</v>
       </c>
       <c r="F51" t="n">
-        <v>2.886904761904762</v>
+        <v>0.05238095238095238</v>
       </c>
       <c r="G51" t="n">
-        <v>0.03235294117647059</v>
+        <v>0.05</v>
       </c>
       <c r="H51" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J51" t="n">
-        <v>4</v>
-      </c>
-      <c r="K51" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2353,27 +2198,24 @@
         <v>45</v>
       </c>
       <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.047311827956989</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.04838709677419355</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1.451612903225806</v>
+      </c>
+      <c r="I52" t="n">
         <v>6</v>
       </c>
-      <c r="E52" t="n">
-        <v>1</v>
-      </c>
-      <c r="F52" t="n">
-        <v>4.047311827956989</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0.04838709677419355</v>
-      </c>
-      <c r="I52" t="n">
-        <v>1.451612903225806</v>
-      </c>
       <c r="J52" t="n">
-        <v>6</v>
-      </c>
-      <c r="K52" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2390,27 +2232,24 @@
         <v>22</v>
       </c>
       <c r="D53" t="n">
-        <v>2.944444444444445</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>2.800865800865801</v>
       </c>
       <c r="F53" t="n">
-        <v>2.800865800865801</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="H53" t="n">
-        <v>0.04761904761904762</v>
+        <v>1</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>5</v>
-      </c>
-      <c r="K53" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2427,27 +2266,24 @@
         <v>39</v>
       </c>
       <c r="D54" t="n">
+        <v>8</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.667692307692308</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.2243589743589743</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I54" t="n">
         <v>5</v>
       </c>
-      <c r="E54" t="n">
-        <v>8</v>
-      </c>
-      <c r="F54" t="n">
-        <v>3.667692307692308</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0.2243589743589743</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="I54" t="n">
-        <v>1.5</v>
-      </c>
       <c r="J54" t="n">
-        <v>5</v>
-      </c>
-      <c r="K54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2464,27 +2300,24 @@
         <v>63</v>
       </c>
       <c r="D55" t="n">
+        <v>9</v>
+      </c>
+      <c r="E55" t="n">
+        <v>4.391891891891892</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.0472972972972973</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1.702702702702703</v>
+      </c>
+      <c r="I55" t="n">
         <v>6</v>
       </c>
-      <c r="E55" t="n">
-        <v>9</v>
-      </c>
-      <c r="F55" t="n">
-        <v>4.391891891891892</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0.0472972972972973</v>
-      </c>
-      <c r="I55" t="n">
-        <v>1.702702702702703</v>
-      </c>
       <c r="J55" t="n">
-        <v>6</v>
-      </c>
-      <c r="K55" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2501,27 +2334,24 @@
         <v>59</v>
       </c>
       <c r="D56" t="n">
+        <v>13</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.805555555555555</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.05947580645161291</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1.84375</v>
+      </c>
+      <c r="I56" t="n">
         <v>5</v>
       </c>
-      <c r="E56" t="n">
-        <v>13</v>
-      </c>
-      <c r="F56" t="n">
-        <v>2.805555555555555</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0.05947580645161291</v>
-      </c>
-      <c r="I56" t="n">
-        <v>1.84375</v>
-      </c>
       <c r="J56" t="n">
-        <v>5</v>
-      </c>
-      <c r="K56" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2538,27 +2368,24 @@
         <v>28</v>
       </c>
       <c r="D57" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>2.705882352941177</v>
       </c>
       <c r="F57" t="n">
-        <v>2.705882352941177</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>0</v>
+        <v>0.03988603988603989</v>
       </c>
       <c r="H57" t="n">
-        <v>0.03988603988603989</v>
+        <v>1.037037037037037</v>
       </c>
       <c r="I57" t="n">
-        <v>1.037037037037037</v>
+        <v>4</v>
       </c>
       <c r="J57" t="n">
-        <v>4</v>
-      </c>
-      <c r="K57" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2575,27 +2402,24 @@
         <v>16</v>
       </c>
       <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.213675213675214</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1.230769230769231</v>
+      </c>
+      <c r="I58" t="n">
         <v>4</v>
       </c>
-      <c r="E58" t="n">
-        <v>2</v>
-      </c>
-      <c r="F58" t="n">
-        <v>2.213675213675214</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0.1025641025641026</v>
-      </c>
-      <c r="I58" t="n">
-        <v>1.230769230769231</v>
-      </c>
       <c r="J58" t="n">
-        <v>4</v>
-      </c>
-      <c r="K58" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2612,27 +2436,24 @@
         <v>67</v>
       </c>
       <c r="D59" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E59" t="n">
-        <v>8</v>
+        <v>2.90625</v>
       </c>
       <c r="F59" t="n">
-        <v>2.90625</v>
+        <v>0.08437500000000001</v>
       </c>
       <c r="G59" t="n">
-        <v>0.05400000000000001</v>
+        <v>0.06754032258064516</v>
       </c>
       <c r="H59" t="n">
-        <v>0.06754032258064516</v>
+        <v>2.09375</v>
       </c>
       <c r="I59" t="n">
-        <v>2.09375</v>
+        <v>5</v>
       </c>
       <c r="J59" t="n">
-        <v>6</v>
-      </c>
-      <c r="K59" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2649,27 +2470,24 @@
         <v>31</v>
       </c>
       <c r="D60" t="n">
-        <v>2.333333333333333</v>
+        <v>9</v>
       </c>
       <c r="E60" t="n">
-        <v>9</v>
+        <v>2.609649122807018</v>
       </c>
       <c r="F60" t="n">
-        <v>2.609649122807018</v>
+        <v>0.1046666666666667</v>
       </c>
       <c r="G60" t="n">
-        <v>0.04361111111111111</v>
+        <v>0.05166666666666667</v>
       </c>
       <c r="H60" t="n">
-        <v>0.05166666666666667</v>
+        <v>1.24</v>
       </c>
       <c r="I60" t="n">
-        <v>1.24</v>
+        <v>4</v>
       </c>
       <c r="J60" t="n">
-        <v>4</v>
-      </c>
-      <c r="K60" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2686,27 +2504,24 @@
         <v>24</v>
       </c>
       <c r="D61" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>3.19047619047619</v>
       </c>
       <c r="F61" t="n">
-        <v>3.19047619047619</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>0.03692307692307693</v>
       </c>
       <c r="H61" t="n">
-        <v>0.03692307692307693</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="I61" t="n">
-        <v>0.9230769230769231</v>
+        <v>5</v>
       </c>
       <c r="J61" t="n">
-        <v>5</v>
-      </c>
-      <c r="K61" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2723,27 +2538,24 @@
         <v>21</v>
       </c>
       <c r="D62" t="n">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>3.091787439613527</v>
       </c>
       <c r="F62" t="n">
-        <v>3.091787439613527</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
+        <v>0.04150197628458498</v>
       </c>
       <c r="H62" t="n">
-        <v>0.04150197628458498</v>
+        <v>0.9130434782608695</v>
       </c>
       <c r="I62" t="n">
-        <v>0.9130434782608695</v>
+        <v>5</v>
       </c>
       <c r="J62" t="n">
-        <v>5</v>
-      </c>
-      <c r="K62" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2760,27 +2572,24 @@
         <v>62</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>4.022167487684729</v>
       </c>
       <c r="F63" t="n">
-        <v>4.022167487684729</v>
+        <v>0.06704980842911877</v>
       </c>
       <c r="G63" t="n">
-        <v>0.06704980842911877</v>
+        <v>0.07635467980295567</v>
       </c>
       <c r="H63" t="n">
-        <v>0.07635467980295567</v>
+        <v>2.137931034482758</v>
       </c>
       <c r="I63" t="n">
-        <v>2.137931034482758</v>
+        <v>6</v>
       </c>
       <c r="J63" t="n">
-        <v>1</v>
-      </c>
-      <c r="K63" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2797,27 +2606,24 @@
         <v>84</v>
       </c>
       <c r="D64" t="n">
-        <v>6.5</v>
+        <v>14</v>
       </c>
       <c r="E64" t="n">
-        <v>14</v>
+        <v>4.055370985603544</v>
       </c>
       <c r="F64" t="n">
-        <v>4.055370985603544</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="G64" t="n">
-        <v>0.04761904761904762</v>
+        <v>0.04651162790697674</v>
       </c>
       <c r="H64" t="n">
-        <v>0.04651162790697674</v>
+        <v>1.953488372093023</v>
       </c>
       <c r="I64" t="n">
-        <v>1.953488372093023</v>
+        <v>6</v>
       </c>
       <c r="J64" t="n">
-        <v>7</v>
-      </c>
-      <c r="K64" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2834,27 +2640,24 @@
         <v>31</v>
       </c>
       <c r="D65" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" t="n">
+        <v>3.489230769230769</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.04769230769230769</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1.192307692307692</v>
+      </c>
+      <c r="I65" t="n">
         <v>6</v>
       </c>
-      <c r="E65" t="n">
-        <v>4</v>
-      </c>
-      <c r="F65" t="n">
-        <v>3.489230769230769</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0.04769230769230769</v>
-      </c>
-      <c r="I65" t="n">
-        <v>1.192307692307692</v>
-      </c>
       <c r="J65" t="n">
-        <v>6</v>
-      </c>
-      <c r="K65" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2871,27 +2674,24 @@
         <v>52</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66" t="n">
-        <v>2</v>
+        <v>2.694736842105264</v>
       </c>
       <c r="F66" t="n">
-        <v>2.694736842105264</v>
+        <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>0.06878306878306878</v>
       </c>
       <c r="H66" t="n">
-        <v>0.06878306878306878</v>
+        <v>1.857142857142857</v>
       </c>
       <c r="I66" t="n">
-        <v>1.857142857142857</v>
+        <v>5</v>
       </c>
       <c r="J66" t="n">
-        <v>1</v>
-      </c>
-      <c r="K66" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2908,27 +2708,24 @@
         <v>12</v>
       </c>
       <c r="D67" t="n">
+        <v>5</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1.785714285714286</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.1729166666666667</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.2142857142857143</v>
+      </c>
+      <c r="H67" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I67" t="n">
         <v>3</v>
       </c>
-      <c r="E67" t="n">
-        <v>5</v>
-      </c>
-      <c r="F67" t="n">
-        <v>1.785714285714286</v>
-      </c>
-      <c r="G67" t="n">
-        <v>0.1729166666666667</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0.2142857142857143</v>
-      </c>
-      <c r="I67" t="n">
-        <v>1.5</v>
-      </c>
       <c r="J67" t="n">
-        <v>3</v>
-      </c>
-      <c r="K67" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2945,27 +2742,24 @@
         <v>41</v>
       </c>
       <c r="D68" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E68" t="n">
-        <v>14</v>
+        <v>2.315018315018315</v>
       </c>
       <c r="F68" t="n">
-        <v>2.315018315018315</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>0</v>
+        <v>0.06307692307692307</v>
       </c>
       <c r="H68" t="n">
-        <v>0.06307692307692307</v>
+        <v>1.576923076923077</v>
       </c>
       <c r="I68" t="n">
-        <v>1.576923076923077</v>
+        <v>6</v>
       </c>
       <c r="J68" t="n">
-        <v>6</v>
-      </c>
-      <c r="K68" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2982,27 +2776,24 @@
         <v>65</v>
       </c>
       <c r="D69" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>4.15686274509804</v>
       </c>
       <c r="F69" t="n">
-        <v>4.15686274509804</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>0</v>
+        <v>0.05793226381461675</v>
       </c>
       <c r="H69" t="n">
-        <v>0.05793226381461675</v>
+        <v>1.911764705882353</v>
       </c>
       <c r="I69" t="n">
-        <v>1.911764705882353</v>
+        <v>6</v>
       </c>
       <c r="J69" t="n">
-        <v>7</v>
-      </c>
-      <c r="K69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3019,27 +2810,24 @@
         <v>35</v>
       </c>
       <c r="D70" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>3.866310160427807</v>
       </c>
       <c r="F70" t="n">
-        <v>3.866310160427807</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>0</v>
+        <v>0.02941176470588235</v>
       </c>
       <c r="H70" t="n">
-        <v>0.02941176470588235</v>
+        <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J70" t="n">
-        <v>7</v>
-      </c>
-      <c r="K70" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3056,27 +2844,24 @@
         <v>40</v>
       </c>
       <c r="D71" t="n">
-        <v>2.833333333333333</v>
+        <v>9</v>
       </c>
       <c r="E71" t="n">
-        <v>9</v>
+        <v>3.457661290322581</v>
       </c>
       <c r="F71" t="n">
-        <v>3.457661290322581</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>0.04032258064516129</v>
       </c>
       <c r="H71" t="n">
-        <v>0.04032258064516129</v>
+        <v>1.25</v>
       </c>
       <c r="I71" t="n">
-        <v>1.25</v>
+        <v>5</v>
       </c>
       <c r="J71" t="n">
-        <v>5</v>
-      </c>
-      <c r="K71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3093,27 +2878,24 @@
         <v>45</v>
       </c>
       <c r="D72" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>2.357894736842105</v>
       </c>
       <c r="F72" t="n">
-        <v>2.357894736842105</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="H72" t="n">
-        <v>0.075</v>
+        <v>1.8</v>
       </c>
       <c r="I72" t="n">
-        <v>1.8</v>
+        <v>4</v>
       </c>
       <c r="J72" t="n">
-        <v>6</v>
-      </c>
-      <c r="K72" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3133,24 +2915,21 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>3.362068965517242</v>
       </c>
       <c r="F73" t="n">
-        <v>3.362068965517242</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>0.06650246305418719</v>
       </c>
       <c r="H73" t="n">
-        <v>0.06650246305418719</v>
+        <v>1.862068965517241</v>
       </c>
       <c r="I73" t="n">
-        <v>1.862068965517241</v>
+        <v>5</v>
       </c>
       <c r="J73" t="n">
-        <v>1</v>
-      </c>
-      <c r="K73" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3167,27 +2946,24 @@
         <v>62</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>3.858064516129032</v>
       </c>
       <c r="F74" t="n">
-        <v>3.858064516129032</v>
+        <v>0.01137096774193548</v>
       </c>
       <c r="G74" t="n">
-        <v>0.01137096774193548</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="H74" t="n">
-        <v>0.06666666666666667</v>
+        <v>2</v>
       </c>
       <c r="I74" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J74" t="n">
-        <v>1</v>
-      </c>
-      <c r="K74" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3204,27 +2980,24 @@
         <v>29</v>
       </c>
       <c r="D75" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>4.009852216748769</v>
       </c>
       <c r="F75" t="n">
-        <v>4.009852216748769</v>
+        <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="H75" t="n">
-        <v>0.03571428571428571</v>
+        <v>1</v>
       </c>
       <c r="I75" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J75" t="n">
-        <v>5</v>
-      </c>
-      <c r="K75" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3241,27 +3014,24 @@
         <v>19</v>
       </c>
       <c r="D76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" t="n">
+        <v>3.192982456140351</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
         <v>4</v>
       </c>
-      <c r="E76" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" t="n">
-        <v>3.192982456140351</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0</v>
-      </c>
-      <c r="H76" t="n">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
       <c r="J76" t="n">
-        <v>4</v>
-      </c>
-      <c r="K76" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3278,27 +3048,24 @@
         <v>48</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E77" t="n">
-        <v>12</v>
+        <v>2.432748538011696</v>
       </c>
       <c r="F77" t="n">
-        <v>2.432748538011696</v>
+        <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>0</v>
+        <v>0.1403508771929824</v>
       </c>
       <c r="H77" t="n">
-        <v>0.1403508771929824</v>
+        <v>2.526315789473684</v>
       </c>
       <c r="I77" t="n">
-        <v>2.526315789473684</v>
+        <v>3</v>
       </c>
       <c r="J77" t="n">
-        <v>1</v>
-      </c>
-      <c r="K77" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3315,27 +3082,24 @@
         <v>50</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>3.732307692307692</v>
       </c>
       <c r="F78" t="n">
-        <v>3.732307692307692</v>
+        <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="H78" t="n">
-        <v>0.07692307692307693</v>
+        <v>1.923076923076923</v>
       </c>
       <c r="I78" t="n">
-        <v>1.923076923076923</v>
+        <v>4</v>
       </c>
       <c r="J78" t="n">
-        <v>1</v>
-      </c>
-      <c r="K78" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3352,27 +3116,24 @@
         <v>44</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>3.30752688172043</v>
       </c>
       <c r="F79" t="n">
-        <v>3.30752688172043</v>
+        <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>0.04731182795698925</v>
       </c>
       <c r="H79" t="n">
-        <v>0.04731182795698925</v>
+        <v>1.419354838709677</v>
       </c>
       <c r="I79" t="n">
-        <v>1.419354838709677</v>
+        <v>4</v>
       </c>
       <c r="J79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K79" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3389,27 +3150,24 @@
         <v>21</v>
       </c>
       <c r="D80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="F80" t="n">
-        <v>2.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>0.04150197628458498</v>
       </c>
       <c r="H80" t="n">
-        <v>0.04150197628458498</v>
+        <v>0.9130434782608695</v>
       </c>
       <c r="I80" t="n">
-        <v>0.9130434782608695</v>
+        <v>4</v>
       </c>
       <c r="J80" t="n">
-        <v>4</v>
-      </c>
-      <c r="K80" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3426,27 +3184,24 @@
         <v>66</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>2.955714285714286</v>
       </c>
       <c r="F81" t="n">
-        <v>2.955714285714286</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>0.04024390243902439</v>
       </c>
       <c r="H81" t="n">
-        <v>0.04024390243902439</v>
+        <v>1.609756097560976</v>
       </c>
       <c r="I81" t="n">
-        <v>1.609756097560976</v>
+        <v>4</v>
       </c>
       <c r="J81" t="n">
-        <v>1</v>
-      </c>
-      <c r="K81" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3463,27 +3218,24 @@
         <v>39</v>
       </c>
       <c r="D82" t="n">
+        <v>16</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4.268115942028985</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.1395833333333333</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.07065217391304347</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="I82" t="n">
         <v>6</v>
       </c>
-      <c r="E82" t="n">
-        <v>16</v>
-      </c>
-      <c r="F82" t="n">
-        <v>4.268115942028985</v>
-      </c>
-      <c r="G82" t="n">
-        <v>0.1395833333333333</v>
-      </c>
-      <c r="H82" t="n">
-        <v>0.07065217391304347</v>
-      </c>
-      <c r="I82" t="n">
-        <v>1.625</v>
-      </c>
       <c r="J82" t="n">
-        <v>6</v>
-      </c>
-      <c r="K82" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3500,27 +3252,24 @@
         <v>34</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>2.964912280701755</v>
       </c>
       <c r="F83" t="n">
-        <v>2.964912280701755</v>
+        <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>0.06159420289855073</v>
       </c>
       <c r="H83" t="n">
-        <v>0.06159420289855073</v>
+        <v>1.416666666666667</v>
       </c>
       <c r="I83" t="n">
-        <v>1.416666666666667</v>
+        <v>4</v>
       </c>
       <c r="J83" t="n">
-        <v>1</v>
-      </c>
-      <c r="K83" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3540,24 +3289,21 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>3.566666666666667</v>
       </c>
       <c r="F84" t="n">
-        <v>3.566666666666667</v>
+        <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="H84" t="n">
-        <v>0.05333333333333334</v>
+        <v>1.28</v>
       </c>
       <c r="I84" t="n">
-        <v>1.28</v>
+        <v>4</v>
       </c>
       <c r="J84" t="n">
-        <v>1</v>
-      </c>
-      <c r="K84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3574,27 +3320,24 @@
         <v>27</v>
       </c>
       <c r="D85" t="n">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>3.083333333333333</v>
       </c>
       <c r="F85" t="n">
-        <v>3.083333333333333</v>
+        <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>0</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="H85" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="I85" t="n">
-        <v>0.9642857142857143</v>
+        <v>4</v>
       </c>
       <c r="J85" t="n">
-        <v>4</v>
-      </c>
-      <c r="K85" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3611,27 +3354,24 @@
         <v>52</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>3.056556346878927</v>
       </c>
       <c r="F86" t="n">
-        <v>3.056556346878927</v>
+        <v>0.04717741935483871</v>
       </c>
       <c r="G86" t="n">
-        <v>0.03179347826086956</v>
+        <v>0.05591397849462366</v>
       </c>
       <c r="H86" t="n">
-        <v>0.05591397849462366</v>
+        <v>1.67741935483871</v>
       </c>
       <c r="I86" t="n">
-        <v>1.67741935483871</v>
+        <v>5</v>
       </c>
       <c r="J86" t="n">
-        <v>1</v>
-      </c>
-      <c r="K86" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3648,27 +3388,24 @@
         <v>10</v>
       </c>
       <c r="D87" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="F87" t="n">
-        <v>1.818181818181818</v>
+        <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>0</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="H87" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="I87" t="n">
-        <v>0.9090909090909091</v>
+        <v>2</v>
       </c>
       <c r="J87" t="n">
-        <v>2</v>
-      </c>
-      <c r="K87" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3685,27 +3422,24 @@
         <v>15</v>
       </c>
       <c r="D88" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>1.944444444444445</v>
       </c>
       <c r="F88" t="n">
-        <v>1.944444444444445</v>
+        <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
+        <v>0.1136363636363636</v>
       </c>
       <c r="H88" t="n">
-        <v>0.1136363636363636</v>
+        <v>1.25</v>
       </c>
       <c r="I88" t="n">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="J88" t="n">
-        <v>3</v>
-      </c>
-      <c r="K88" t="n">
         <v>2</v>
       </c>
     </row>
@@ -3722,27 +3456,24 @@
         <v>25</v>
       </c>
       <c r="D89" t="n">
+        <v>2</v>
+      </c>
+      <c r="E89" t="n">
+        <v>3.147186147186147</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.04557416267942584</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.05411255411255411</v>
+      </c>
+      <c r="H89" t="n">
+        <v>1.136363636363636</v>
+      </c>
+      <c r="I89" t="n">
         <v>6</v>
       </c>
-      <c r="E89" t="n">
-        <v>2</v>
-      </c>
-      <c r="F89" t="n">
-        <v>3.147186147186147</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0.04557416267942584</v>
-      </c>
-      <c r="H89" t="n">
-        <v>0.05411255411255411</v>
-      </c>
-      <c r="I89" t="n">
-        <v>1.136363636363636</v>
-      </c>
       <c r="J89" t="n">
-        <v>6</v>
-      </c>
-      <c r="K89" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3759,27 +3490,24 @@
         <v>28</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" t="n">
-        <v>1</v>
+        <v>3.891737891737892</v>
       </c>
       <c r="F90" t="n">
-        <v>3.891737891737892</v>
+        <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>0.03988603988603989</v>
       </c>
       <c r="H90" t="n">
-        <v>0.03988603988603989</v>
+        <v>1.037037037037037</v>
       </c>
       <c r="I90" t="n">
-        <v>1.037037037037037</v>
+        <v>5</v>
       </c>
       <c r="J90" t="n">
-        <v>1</v>
-      </c>
-      <c r="K90" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3796,27 +3524,24 @@
         <v>18</v>
       </c>
       <c r="D91" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E91" t="n">
-        <v>2</v>
+        <v>2.992647058823529</v>
       </c>
       <c r="F91" t="n">
-        <v>2.992647058823529</v>
+        <v>0.02908496732026144</v>
       </c>
       <c r="G91" t="n">
-        <v>0.02908496732026144</v>
+        <v>0.06617647058823529</v>
       </c>
       <c r="H91" t="n">
-        <v>0.06617647058823529</v>
+        <v>1.058823529411765</v>
       </c>
       <c r="I91" t="n">
-        <v>1.058823529411765</v>
+        <v>4</v>
       </c>
       <c r="J91" t="n">
-        <v>5</v>
-      </c>
-      <c r="K91" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3833,27 +3558,24 @@
         <v>41</v>
       </c>
       <c r="D92" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" t="n">
+        <v>3.883870967741935</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0.04408602150537634</v>
+      </c>
+      <c r="H92" t="n">
+        <v>1.32258064516129</v>
+      </c>
+      <c r="I92" t="n">
         <v>5</v>
       </c>
-      <c r="E92" t="n">
-        <v>1</v>
-      </c>
-      <c r="F92" t="n">
-        <v>3.883870967741935</v>
-      </c>
-      <c r="G92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H92" t="n">
-        <v>0.04408602150537634</v>
-      </c>
-      <c r="I92" t="n">
-        <v>1.32258064516129</v>
-      </c>
       <c r="J92" t="n">
-        <v>5</v>
-      </c>
-      <c r="K92" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>